<commit_message>
made changes based on Elizabeth request
</commit_message>
<xml_diff>
--- a/demo_data/flowrate.xlsx
+++ b/demo_data/flowrate.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sccwrp.sharepoint.com/sites/Staff/Shared Documents/P Drive/Data/DuyNguyen/Projects/bioretention_rain/demo_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{E1E1FAC7-CE81-40D3-BA68-902FCADE7445}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{76B46238-3B1E-4668-B817-6015448E786F}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:1_{E1E1FAC7-CE81-40D3-BA68-902FCADE7445}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0C34DCDB-9575-48B0-A274-9A2572334130}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="165" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="inflow" sheetId="1" r:id="rId1"/>
+    <sheet name="inflow1" sheetId="1" r:id="rId1"/>
     <sheet name="inflow2" sheetId="2" r:id="rId2"/>
-    <sheet name="outflow" sheetId="3" r:id="rId3"/>
-    <sheet name="bypass" sheetId="4" r:id="rId4"/>
+    <sheet name="bypass" sheetId="3" r:id="rId3"/>
+    <sheet name="outflow" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
@@ -436,8 +436,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B1972"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -47813,8 +47813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B1971"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
updated ui aesthetics, added inflow/outflow validation, corrected outflow_time check, updated templates/demo data
</commit_message>
<xml_diff>
--- a/demo_data/flowrate.xlsx
+++ b/demo_data/flowrate.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sccwrp.sharepoint.com/sites/Staff/Shared Documents/P Drive/Data/DuyNguyen/Projects/rainfall_flow_calculator_shiny/demo_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sccwrp.sharepoint.com/sites/Staff/Shared Documents/P Drive/Data/PartTimers/Nick Lombardo/Bioretention/rainfall_flow_analysis/demo_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="13_ncr:1_{E1E1FAC7-CE81-40D3-BA68-902FCADE7445}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9B22408D-E15A-4C48-B71D-6ED81162DA28}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="13_ncr:1_{E1E1FAC7-CE81-40D3-BA68-902FCADE7445}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5BF7B3AA-2E87-4AA7-8037-C7418B9588EA}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -127,14 +127,14 @@
       <xdr:col>13</xdr:col>
       <xdr:colOff>304799</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1">
+        <xdr:cNvPr id="3" name="TextBox 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F4B02833-6773-437E-9902-B0932C04582E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{55B87DA2-024C-4C78-8763-F6B389A9A316}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -143,7 +143,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="8229599" cy="9791700"/>
+          <a:ext cx="8229599" cy="9772650"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -224,7 +224,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>The application supports two types of analysis: Rainfall Analysis and Flow Analysis. In the zip package that </a:t>
+            <a:t>The application supports two types of analysis: Rainfall Analysis and Flow Analysis.</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -281,7 +281,15 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>Demo data is available for flow analysis under demo_data folder.</a:t>
+            <a:t>Demo data is provided</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> on the instructions tab of the application</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>.</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -347,7 +355,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>IMPORTANT: If any of the flow data types are not applicable, leave the corresponding tab blank. Do not modify the columns or the tab names.</a:t>
+            <a:t>IMPORTANT: If any of the flow data types are not applicable, leave the corresponding tab blank. Do not modify the column names or the tab names.</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -355,9 +363,44 @@
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>Demo data is available for flow analysis under demo_data folder.</a:t>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Demo data is provided</a:t>
           </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> on the instructions tab of the application</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:endParaRPr lang="en-US" sz="1100"/>
@@ -764,9 +807,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EE88C01-577A-4903-8B8F-8FB963800B71}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
@@ -63940,15 +63981,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000C0FD75001275F4DBA43EB7BE58C8A34" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="21cacd0d90dbd8beb6fc12ad84d4cd0e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="02ea596c-bf3f-4512-ad68-024a720c79b2" xmlns:ns3="959569b2-1f16-4dd0-b5ed-bb064e5cd07e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5b418c8325abc32123734ac979891270" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -64208,15 +64240,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6636DA7F-7D61-4910-9C4D-7AB6320A82E3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1DBDA20A-1402-4484-A75F-CE3A1FB4E261}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -64234,4 +64267,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6636DA7F-7D61-4910-9C4D-7AB6320A82E3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>